<commit_message>
observable for symptomas and renderer for weekly programme
</commit_message>
<xml_diff>
--- a/BugsLog.xlsx
+++ b/BugsLog.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38320" windowHeight="21140" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Bugs" sheetId="1" r:id="rId1"/>
+    <sheet name="Improvements" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>Bugs</t>
   </si>
@@ -49,6 +50,12 @@
   </si>
   <si>
     <t>Check array that is used for companions' creation: how many instances of 'companions' are created? Which instance should be modified? Will have to change with companion-selection -&gt; going to search into FB Friends (then will be friendSearched/filtered/Selected and not CompanionSearched/filtered/Selected); then will add the selected friends in an array (in companion-element.component) that displays the companions from the database. Hence, ngOnInit of companion-selection.component intialises the array from the service that goes into the database (same for ngOnInit of companion-element and companions-creation) =&gt; the service creates the array that will be displayed in all other components. Button validate updates the companions' array from the database. Not possible to do before Facebook connection because search bar needs to search somewhere. Careful with the formula of the service that only provides a copy of the array, not the actual array (which is why we can always delete and add companions but always get access to the 3 companions created in the service)</t>
+  </si>
+  <si>
+    <t>How not to replicate code between companion-creation.component and companion-management.component</t>
+  </si>
+  <si>
+    <t>Improvements</t>
   </si>
 </sst>
 </file>
@@ -97,8 +104,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -113,17 +124,21 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -455,7 +470,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
@@ -521,4 +536,46 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="2" spans="2:3">
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3">
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3">
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>